<commit_message>
had to change id
</commit_message>
<xml_diff>
--- a/Web/db_data/storages.xlsx
+++ b/Web/db_data/storages.xlsx
@@ -174,15 +174,15 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="0" width="10.56"/>
   </cols>
   <sheetData>
@@ -205,7 +205,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -222,7 +222,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -239,7 +239,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -256,7 +256,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>

</xml_diff>